<commit_message>
se agrego el modulo de cargar xml de recepcion de transferencia de sucursal
</commit_message>
<xml_diff>
--- a/diccionario.xlsx
+++ b/diccionario.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anton\source\repos\caja\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14580B0F-9609-44BF-B773-7130E1A6569D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B5BA6D0-ADF4-459E-BE50-A9705690A45E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{003534D2-26D7-45B8-9722-D21F20769DC0}"/>
   </bookViews>
   <sheets>
     <sheet name="tbakardez" sheetId="1" r:id="rId1"/>
+    <sheet name="tbatraspasos" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>Campo</t>
   </si>
@@ -48,20 +49,35 @@
     <t>VARCHAR(2)</t>
   </si>
   <si>
-    <t>E= Entrada, S= salida, A= Ajuste, V= Venta, T= Traspaso, C= Compra</t>
+    <t>tipo</t>
+  </si>
+  <si>
+    <t>varchar</t>
+  </si>
+  <si>
+    <t>E= Envio,  R= Recepcion</t>
+  </si>
+  <si>
+    <t>E= Entrada, S= salida, A= Ajuste, V= Venta, T= Traspaso, C= Compra, I=Traspaso Ingreso</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -84,7 +100,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -92,6 +108,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -409,7 +426,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -425,7 +442,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -433,7 +450,48 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6131B79A-9B63-42FD-9AA8-894BB4C9C4E2}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>5</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se afecta inventario con la cancelacion del ticket
</commit_message>
<xml_diff>
--- a/diccionario.xlsx
+++ b/diccionario.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anton\source\repos\caja\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B5BA6D0-ADF4-459E-BE50-A9705690A45E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF9402BB-3E19-429D-8C82-E11B73FF6413}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{003534D2-26D7-45B8-9722-D21F20769DC0}"/>
   </bookViews>
@@ -58,7 +58,7 @@
     <t>E= Envio,  R= Recepcion</t>
   </si>
   <si>
-    <t>E= Entrada, S= salida, A= Ajuste, V= Venta, T= Traspaso, C= Compra, I=Traspaso Ingreso</t>
+    <t>E= Entrada, S= salida, A= Ajuste, V= Venta, T= Traspaso, C= Compra, I=Traspaso Ingreso,         D=Cancelar Venta</t>
   </si>
 </sst>
 </file>
@@ -426,10 +426,13 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="11.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -442,7 +445,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="165" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>

</xml_diff>